<commit_message>
update phan cong cong viec
</commit_message>
<xml_diff>
--- a/Phan-cong-project-web-1.xlsx
+++ b/Phan-cong-project-web-1.xlsx
@@ -159,10 +159,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -189,22 +189,100 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,114 +297,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -361,55 +361,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,7 +517,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,115 +535,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -579,6 +579,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -594,11 +603,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,8 +645,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,30 +668,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -679,7 +679,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -697,130 +697,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -916,48 +916,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>261620</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7353300" y="182880"/>
-          <a:ext cx="10431780" cy="5509895"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
       <xdr:colOff>29845</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -970,7 +928,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1012,7 +970,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1302,8 +1260,8 @@
   <sheetPr/>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1314,7 +1272,7 @@
     <col min="4" max="4" width="26.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" customHeight="1" spans="1:12">
+    <row r="1" customHeight="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1288,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" customFormat="1" customHeight="1" spans="1:12">
+    <row r="2" customHeight="1" spans="1:12">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1344,7 +1302,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" customFormat="1" customHeight="1" spans="1:12">
+    <row r="3" customHeight="1" spans="1:12">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1358,7 +1316,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" customFormat="1" customHeight="1" spans="1:12">
+    <row r="4" customHeight="1" spans="1:12">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1372,7 +1330,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" customFormat="1" ht="31.2" customHeight="1" spans="1:4">
+    <row r="5" ht="31.2" customHeight="1" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1386,7 +1344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="1" ht="34.8" customHeight="1" spans="1:4">
+    <row r="6" ht="34.8" customHeight="1" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1400,7 +1358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="49.05" customHeight="1" spans="1:4">
+    <row r="7" ht="49.05" customHeight="1" spans="1:4">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1410,7 +1368,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" customFormat="1" ht="45" customHeight="1" spans="1:4">
+    <row r="8" ht="45" customHeight="1" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1424,7 +1382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="1" ht="31.8" customHeight="1" spans="1:4">
+    <row r="9" ht="31.8" customHeight="1" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
@@ -1438,7 +1396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="28.8" customHeight="1" spans="1:4">
+    <row r="10" ht="28.8" customHeight="1" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -1452,7 +1410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="37.8" customHeight="1" spans="1:4">
+    <row r="11" ht="37.8" customHeight="1" spans="1:4">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
@@ -1466,7 +1424,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="31.8" customHeight="1" spans="1:4">
+    <row r="12" ht="31.8" customHeight="1" spans="1:4">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -1480,7 +1438,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="1" ht="38.4" customHeight="1" spans="1:4">
+    <row r="13" ht="38.4" customHeight="1" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
@@ -1494,7 +1452,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="41.4" customHeight="1" spans="1:4">
+    <row r="14" ht="41.4" customHeight="1" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1508,7 +1466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="1" ht="58.2" customHeight="1" spans="1:4">
+    <row r="15" ht="58.2" customHeight="1" spans="1:4">
       <c r="A15" s="8" t="s">
         <v>28</v>
       </c>
@@ -1522,7 +1480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="1" ht="37.2" customHeight="1" spans="1:4">
+    <row r="16" ht="37.2" customHeight="1" spans="1:4">
       <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
@@ -1536,7 +1494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="57.6" customHeight="1" spans="1:4">
+    <row r="17" ht="57.6" customHeight="1" spans="1:4">
       <c r="A17" s="8" t="s">
         <v>31</v>
       </c>
@@ -1550,7 +1508,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="52.8" customHeight="1" spans="1:4">
+    <row r="18" ht="52.8" customHeight="1" spans="1:4">
       <c r="A18" s="8" t="s">
         <v>32</v>
       </c>
@@ -1564,7 +1522,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" customFormat="1" ht="38.4" customHeight="1" spans="1:4">
+    <row r="19" ht="38.4" customHeight="1" spans="1:4">
       <c r="A19" s="8" t="s">
         <v>34</v>
       </c>
@@ -1578,7 +1536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="29.4" customHeight="1" spans="1:4">
+    <row r="20" ht="29.4" customHeight="1" spans="1:4">
       <c r="A20" s="8" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
update phan cong cong viec -v3
</commit_message>
<xml_diff>
--- a/Phan-cong-project-web-1.xlsx
+++ b/Phan-cong-project-web-1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-nhom-C-chuyen-de-web1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>DỰ ÁN THUÊ KHÁCH SẠN</t>
   </si>
@@ -123,27 +118,30 @@
     <t>Laravel</t>
   </si>
   <si>
+    <t>Trung(80%)</t>
+  </si>
+  <si>
+    <t>Chức năng hiển thị và phân trang: khách sạn, địa điểm thuê</t>
+  </si>
+  <si>
+    <t>Trung(Đã hoàn thành)</t>
+  </si>
+  <si>
+    <t>Chức năng thêm khách sạn vào trang yêu thích</t>
+  </si>
+  <si>
+    <t>Chức năng trả dữ liệu khi user điền đầy đủ thông tin khách sạn</t>
+  </si>
+  <si>
+    <t>Chức năng bình luận, đánh giá cho user đã thuê qua khách sạn đó</t>
+  </si>
+  <si>
+    <t>7-8 tiếng</t>
+  </si>
+  <si>
     <t>Trung</t>
   </si>
   <si>
-    <t>Chức năng hiển thị và phân trang: khách sạn, địa điểm thuê</t>
-  </si>
-  <si>
-    <t>Lâm</t>
-  </si>
-  <si>
-    <t>Chức năng thêm khách sạn vào trang yêu thích</t>
-  </si>
-  <si>
-    <t>Chức năng trả dữ liệu khi user điền đầy đủ thông tin khách sạn</t>
-  </si>
-  <si>
-    <t>Chức năng bình luận, đánh giá cho user đã thuê qua khách sạn đó</t>
-  </si>
-  <si>
-    <t>7-8 tiếng</t>
-  </si>
-  <si>
     <t>Chức năng xác nhận tài khoản qua mail</t>
   </si>
   <si>
@@ -157,19 +155,19 @@
   </si>
   <si>
     <t>30 phút</t>
-  </si>
-  <si>
-    <t>Trung(Đã hoàn thành)</t>
-  </si>
-  <si>
-    <t>Trung(80%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,15 +191,159 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,7 +352,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39991454817346722"/>
+        <fgColor theme="8" tint="0.399914548173467"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,8 +362,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -253,12 +581,257 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -271,40 +844,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -326,7 +937,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -368,7 +979,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -644,302 +1255,302 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="29.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="28.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="26.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" customHeight="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="31.2" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:12">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:12">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:12">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" ht="31.2" customHeight="1" spans="1:4">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="34.799999999999997" customHeight="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" ht="34.8" customHeight="1" spans="1:4">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="49.05" customHeight="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" ht="49.05" customHeight="1" spans="1:4">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="45" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" ht="45" customHeight="1" spans="1:4">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="31.8" customHeight="1">
-      <c r="A9" s="6" t="s">
+    <row r="9" ht="31.8" customHeight="1" spans="1:4">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" customHeight="1">
-      <c r="A10" s="6" t="s">
+    <row r="10" ht="28.8" customHeight="1" spans="1:4">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="37.799999999999997" customHeight="1">
-      <c r="A11" s="6" t="s">
+    <row r="11" ht="37.8" customHeight="1" spans="1:4">
+      <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="31.8" customHeight="1">
-      <c r="A12" s="6" t="s">
+    <row r="12" ht="31.8" customHeight="1" spans="1:4">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="38.4" customHeight="1">
-      <c r="A13" s="6" t="s">
+    <row r="13" ht="38.4" customHeight="1" spans="1:4">
+      <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="41.4" customHeight="1">
-      <c r="A14" s="6" t="s">
+    <row r="14" ht="41.4" customHeight="1" spans="1:4">
+      <c r="A14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="58.2" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="D14" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" ht="58.2" customHeight="1" spans="1:4">
+      <c r="A15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" ht="37.2" customHeight="1" spans="1:4">
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" ht="57.6" customHeight="1" spans="1:4">
+      <c r="A17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" ht="52.8" customHeight="1" spans="1:4">
+      <c r="A18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" ht="38.4" customHeight="1" spans="1:4">
+      <c r="A19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" ht="29.4" customHeight="1" spans="1:4">
+      <c r="A20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="37.200000000000003" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="57.6" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="52.8" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="38.4" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="29.4" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -949,7 +1560,8 @@
     <mergeCell ref="A1:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>